<commit_message>
Fixes in user vehicles
</commit_message>
<xml_diff>
--- a/m100_Tools_And_Helpers/User Vehicles.xlsx
+++ b/m100_Tools_And_Helpers/User Vehicles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robsc\source\repos\LusasNoteBooks\m100_Tools_And_Helpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9971B15D-CB25-48D7-9623-34CD42B003DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AAF1C6-05BB-46F1-8E31-5D29CF34F01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2184" yWindow="3336" windowWidth="20616" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicles" sheetId="2" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Widths</t>
   </si>
   <si>
-    <t>N,m,kg,C,s</t>
-  </si>
-  <si>
     <t>MyVehicle1</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Double wheel  in last axle posiiton</t>
   </si>
   <si>
-    <t>0|5|10|12</t>
-  </si>
-  <si>
     <t>1.5|1.5|2|2|2.5</t>
   </si>
   <si>
@@ -77,7 +71,13 @@
     <t>Spacings</t>
   </si>
   <si>
-    <t>0|5|10|12|0</t>
+    <t>N,m,kg,s,C</t>
+  </si>
+  <si>
+    <t>0|2|5|2</t>
+  </si>
+  <si>
+    <t>0|2|5|2|0</t>
   </si>
 </sst>
 </file>
@@ -440,17 +440,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -458,24 +458,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -485,24 +485,24 @@
         <v>2.2|2.2|2.2|2.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>